<commit_message>
revisao, melhorias e mudancas
revisao de alguns nomes
melhoras de algumas traducoes
mudancas de alguns conceitos
</commit_message>
<xml_diff>
--- a/Traduzido/PTBR/Lang/PTBR/Dialog/Drama/ashland.xlsx
+++ b/Traduzido/PTBR/Lang/PTBR/Dialog/Drama/ashland.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Dialog\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Dialog\Drama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3092E2EE-8F57-4AED-B1A2-58EA4BACF134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD531FB-9430-436C-89C3-D0EC268132A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="376">
   <si>
     <t>step</t>
   </si>
@@ -1119,11 +1119,6 @@
 Inicialmente, a variedade de itens que você pode criar é limitada, mas conforme obtém novas receitas durante sua jornada, poderá fabricar uma grande variedade de itens úteis.</t>
   </si>
   <si>
-    <t>Ao fabricar itens, você pode usar ingredientes da sua mochila e de contêineres distantes, desde que pertençam a você._x000D_
-_x000D_
-Se você não tiver as habilidades necessárias para a criação, consumirá muita energia. Por isso, é recomendável aprimorar suas habilidades criando itens simples antes de tentar receitas de nível avançado.</t>
-  </si>
-  <si>
     <t>(Chegando!)</t>
   </si>
   <si>
@@ -1380,21 +1375,6 @@
 Você pode usá-las para pagar treinadores de habilidades na cidade e aprender novas técnicas.</t>
   </si>
   <si>
-    <t>Enquanto constrói sua base aqui, você precisa conhecer o "container compartilhado"._x000D_
-_x000D_
-O container compartilhado é um item essencial para que seus moradores possam viver e trabalhar. Preste atenção, pois vou explicar apenas uma vez.</t>
-  </si>
-  <si>
-    <t>Contêineres como caixotes e barris possuem um sistema de "permissões". Normalmente, apenas você pode mover itens dentro e fora de um contêiner, mas é possível transformá-lo em um container compartilhado clicando no ícone de "Cadeado" no lado direito do contêiner._x000D_
-_x000D_
-Os containers compartilhados podem ser acessados pelos moradores e membros do grupo. Quem estiver com fome poderá procurar comida neles e, se encontrar um bom equipamento, pode pegá-lo. Caso haja materiais necessários para o trabalho, eles serão consumidos automaticamente.</t>
-  </si>
-  <si>
-    <t>Além disso, fique atento à capacidade restante do container compartilhado, pois os moradores podem entregar produtos de trabalho ou itens que encontrarem._x000D_
-_x000D_
-Vou te dar esta caixa como recompensa por esta missão. Coloque-a no chão e tente transformá-la em um "container compartilhado".</t>
-  </si>
-  <si>
     <t>Parece que você configurou um container compartilhado com sucesso._x000D_
 _x000D_
 Ao alterar as configurações dos containers, você também pode criar containers que são usados com prioridade ou que permitem apenas a movimentação de itens de uma determinada categoria. Você pode testar isso mais tarde, quando precisar organizar os suprimentos da base.</t>
@@ -1483,6 +1463,38 @@
   </si>
   <si>
     <t>Tenho algo que gostaria de perguntar.</t>
+  </si>
+  <si>
+    <t>Enquanto constrói sua base aqui, você precisa conhecer o "Caixa Compartilhada".
+O container compartilhado é um item essencial para que seus moradores possam viver e trabalhar. Preste atenção, pois vou explicar apenas uma vez.</t>
+  </si>
+  <si>
+    <t>Enquanto constrói sua base aqui, você precisa conhecer o "Caixa Compartilhada"._x000D_
+_x000D_
+O container compartilhado é um item essencial para que seus moradores possam viver e trabalhar. Preste atenção, pois vou explicar apenas uma vez.</t>
+  </si>
+  <si>
+    <t>Além disso, fique atento à capacidade restante do container compartilhado, pois os moradores podem entregar produtos de trabalho ou itens que encontrarem._x000D_
+_x000D_
+Vou te dar esta caixa como recompensa por esta missão. Coloque-a no chão e tente transformá-la em um "Caixa Compartilhada".</t>
+  </si>
+  <si>
+    <t>Armazenamentos como Caixotes, Baús e Barris possuem um sistema de "permissões". Normalmente, apenas você pode mover itens dentro e fora de um contêiner, mas é possível transformá-lo em um container compartilhado clicando no ícone de "Cadeado" no lado direito do contêiner.
+Os containers compartilhados podem ser acessados pelos moradores e membros do grupo. Quem estiver com fome poderá procurar comida neles e, se encontrar um bom equipamento, pode pegá-lo. Caso haja materiais necessários para o trabalho, eles serão consumidos automaticamente.</t>
+  </si>
+  <si>
+    <t>Armazenamentos como Caixotes, Baús e Barris possuem um sistema de "permissões". Normalmente, apenas você pode mover itens dentro e fora de um contêiner, mas é possível transformá-lo em um container compartilhado clicando no ícone de "Cadeado" no lado direito do contêiner._x000D_
+_x000D_
+Os containers compartilhados podem ser acessados pelos moradores e membros do grupo. Quem estiver com fome poderá procurar comida neles e, se encontrar um bom equipamento, pode pegá-lo. Caso haja materiais necessários para o trabalho, eles serão consumidos automaticamente.</t>
+  </si>
+  <si>
+    <t>Ao fabricar itens, você pode usar ingredientes da sua Mochila, Caixas, Baús e de Contêineres distantes, desde que pertençam a você.
+Se você não tiver as habilidades necessárias para a criação, consumirá muita energia. Por isso, é recomendável aprimorar suas habilidades criando itens simples antes de tentar receitas de nível avançado.</t>
+  </si>
+  <si>
+    <t>Ao fabricar itens, você pode usar ingredientes da sua Mochila, Caixas, Baús e de Contêineres distantes, desde que pertençam a você._x000D_
+_x000D_
+Se você não tiver as habilidades necessárias para a criação, consumirá muita energia. Por isso, é recomendável aprimorar suas habilidades criando itens simples antes de tentar receitas de nível avançado.</t>
   </si>
 </sst>
 </file>
@@ -1787,9 +1799,9 @@
   <dimension ref="A1:L372"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomLeft" activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="16.5"/>
@@ -1897,7 +1909,7 @@
         <v>117</v>
       </c>
       <c r="J15" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="K15" t="s">
         <v>22</v>
@@ -1917,7 +1929,7 @@
         <v>118</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="K16" t="s">
         <v>25</v>
@@ -1934,7 +1946,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>27</v>
@@ -1962,7 +1974,7 @@
         <v>2</v>
       </c>
       <c r="J20" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="K20" t="s">
         <v>31</v>
@@ -1985,7 +1997,7 @@
         <v>3</v>
       </c>
       <c r="J21" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="K21" t="s">
         <v>34</v>
@@ -2005,7 +2017,7 @@
         <v>4</v>
       </c>
       <c r="J22" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="K22" t="s">
         <v>36</v>
@@ -2025,7 +2037,7 @@
         <v>5</v>
       </c>
       <c r="J23" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="K23" t="s">
         <v>38</v>
@@ -2815,13 +2827,13 @@
         <v>38</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>295</v>
+        <v>374</v>
       </c>
       <c r="K99" s="3" t="s">
         <v>113</v>
       </c>
       <c r="L99" s="3" t="s">
-        <v>295</v>
+        <v>375</v>
       </c>
     </row>
     <row r="100" spans="1:12">
@@ -2853,13 +2865,13 @@
         <v>39</v>
       </c>
       <c r="J105" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K105" t="s">
         <v>116</v>
       </c>
       <c r="L105" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="106" spans="1:12">
@@ -2891,13 +2903,13 @@
         <v>40</v>
       </c>
       <c r="J110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K110" s="3" t="s">
         <v>119</v>
       </c>
       <c r="L110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:12">
@@ -2931,13 +2943,13 @@
         <v>41</v>
       </c>
       <c r="J116" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K116" s="3" t="s">
         <v>122</v>
       </c>
       <c r="L116" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="117" spans="1:12">
@@ -2971,13 +2983,13 @@
         <v>42</v>
       </c>
       <c r="J122" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K122" t="s">
         <v>116</v>
       </c>
       <c r="L122" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="123" spans="1:12">
@@ -2998,13 +3010,13 @@
         <v>43</v>
       </c>
       <c r="J133" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K133" s="3" t="s">
         <v>125</v>
       </c>
       <c r="L133" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="134" spans="1:12" ht="82.5">
@@ -3012,13 +3024,13 @@
         <v>44</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K134" s="3" t="s">
         <v>126</v>
       </c>
       <c r="L134" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -3036,13 +3048,13 @@
         <v>45</v>
       </c>
       <c r="J138" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K138" s="3" t="s">
         <v>127</v>
       </c>
       <c r="L138" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -3060,13 +3072,13 @@
         <v>47</v>
       </c>
       <c r="J142" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K142" s="3" t="s">
         <v>128</v>
       </c>
       <c r="L142" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="143" spans="1:12" ht="198">
@@ -3074,13 +3086,13 @@
         <v>48</v>
       </c>
       <c r="J143" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K143" s="3" t="s">
         <v>129</v>
       </c>
       <c r="L143" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="144" spans="1:12" ht="99">
@@ -3088,13 +3100,13 @@
         <v>49</v>
       </c>
       <c r="J144" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K144" s="3" t="s">
         <v>130</v>
       </c>
       <c r="L144" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="145" spans="1:12">
@@ -3112,13 +3124,13 @@
         <v>50</v>
       </c>
       <c r="J148" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="K148" s="3" t="s">
         <v>131</v>
       </c>
       <c r="L148" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="149" spans="1:12" ht="148.5">
@@ -3126,13 +3138,13 @@
         <v>51</v>
       </c>
       <c r="J149" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="K149" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L149" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="150" spans="1:12" ht="132">
@@ -3140,13 +3152,13 @@
         <v>52</v>
       </c>
       <c r="J150" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K150" s="3" t="s">
         <v>133</v>
       </c>
       <c r="L150" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="151" spans="1:12">
@@ -3164,13 +3176,13 @@
         <v>53</v>
       </c>
       <c r="J156" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K156" s="3" t="s">
         <v>134</v>
       </c>
       <c r="L156" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="198">
@@ -3178,13 +3190,13 @@
         <v>54</v>
       </c>
       <c r="J157" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K157" s="3" t="s">
         <v>135</v>
       </c>
       <c r="L157" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="159" spans="1:12">
@@ -3202,13 +3214,13 @@
         <v>55</v>
       </c>
       <c r="J162" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K162" s="3" t="s">
         <v>136</v>
       </c>
       <c r="L162" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="163" spans="1:12" ht="99">
@@ -3216,13 +3228,13 @@
         <v>56</v>
       </c>
       <c r="J163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K163" s="3" t="s">
         <v>137</v>
       </c>
       <c r="L163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:12">
@@ -3384,13 +3396,13 @@
         <v>62</v>
       </c>
       <c r="J208" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K208" s="3" t="s">
         <v>159</v>
       </c>
       <c r="L208" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="209" spans="1:12">
@@ -3398,13 +3410,13 @@
         <v>63</v>
       </c>
       <c r="J209" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K209" t="s">
         <v>160</v>
       </c>
       <c r="L209" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="210" spans="1:12">
@@ -3430,13 +3442,13 @@
         <v>64</v>
       </c>
       <c r="J215" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K215" s="3" t="s">
         <v>163</v>
       </c>
       <c r="L215" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="216" spans="1:12" ht="99">
@@ -3444,13 +3456,13 @@
         <v>65</v>
       </c>
       <c r="J216" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K216" s="3" t="s">
         <v>164</v>
       </c>
       <c r="L216" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="217" spans="1:12">
@@ -3458,13 +3470,13 @@
         <v>66</v>
       </c>
       <c r="J217" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K217" t="s">
         <v>165</v>
       </c>
       <c r="L217" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="218" spans="1:12">
@@ -3472,13 +3484,13 @@
         <v>67</v>
       </c>
       <c r="J218" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K218" t="s">
         <v>166</v>
       </c>
       <c r="L218" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="219" spans="1:12">
@@ -3501,13 +3513,13 @@
         <v>68</v>
       </c>
       <c r="J222" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K222" s="3" t="s">
         <v>168</v>
       </c>
       <c r="L222" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="223" spans="1:12">
@@ -3525,13 +3537,13 @@
         <v>69</v>
       </c>
       <c r="J226" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K226" s="3" t="s">
         <v>170</v>
       </c>
       <c r="L226" s="3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="227" spans="1:12" ht="148.5">
@@ -3539,13 +3551,13 @@
         <v>70</v>
       </c>
       <c r="J227" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="K227" s="3" t="s">
         <v>171</v>
       </c>
       <c r="L227" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="228" spans="1:12" ht="82.5">
@@ -3553,13 +3565,13 @@
         <v>71</v>
       </c>
       <c r="J228" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K228" s="3" t="s">
         <v>172</v>
       </c>
       <c r="L228" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="229" spans="1:12">
@@ -3600,13 +3612,13 @@
         <v>72</v>
       </c>
       <c r="J239" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K239" s="3" t="s">
         <v>177</v>
       </c>
       <c r="L239" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="240" spans="1:12">
@@ -3622,13 +3634,13 @@
         <v>73</v>
       </c>
       <c r="J241" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K241" s="3" t="s">
         <v>179</v>
       </c>
       <c r="L241" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="242" spans="1:12">
@@ -3662,13 +3674,13 @@
         <v>74</v>
       </c>
       <c r="J248" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K248" s="3" t="s">
         <v>183</v>
       </c>
       <c r="L248" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="249" spans="1:12">
@@ -3708,13 +3720,13 @@
         <v>75</v>
       </c>
       <c r="J253" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="K253" s="3" t="s">
         <v>190</v>
       </c>
       <c r="L253" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="254" spans="1:12">
@@ -3722,13 +3734,13 @@
         <v>76</v>
       </c>
       <c r="J254" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="K254" t="s">
         <v>191</v>
       </c>
       <c r="L254" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="66">
@@ -3736,13 +3748,13 @@
         <v>77</v>
       </c>
       <c r="J255" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K255" s="3" t="s">
         <v>192</v>
       </c>
       <c r="L255" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="115.5">
@@ -3750,13 +3762,13 @@
         <v>78</v>
       </c>
       <c r="J256" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K256" s="3" t="s">
         <v>193</v>
       </c>
       <c r="L256" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="257" spans="1:12" ht="132">
@@ -3764,13 +3776,13 @@
         <v>79</v>
       </c>
       <c r="J257" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K257" s="3" t="s">
         <v>194</v>
       </c>
       <c r="L257" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="258" spans="1:12" ht="82.5">
@@ -3778,13 +3790,13 @@
         <v>80</v>
       </c>
       <c r="J258" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K258" s="3" t="s">
         <v>195</v>
       </c>
       <c r="L258" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="260" spans="1:12" ht="132">
@@ -3792,13 +3804,13 @@
         <v>81</v>
       </c>
       <c r="J260" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K260" s="3" t="s">
         <v>196</v>
       </c>
       <c r="L260" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="263" spans="1:12">
@@ -3829,13 +3841,13 @@
         <v>82</v>
       </c>
       <c r="J271" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K271" s="3" t="s">
         <v>199</v>
       </c>
       <c r="L271" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="272" spans="1:12" ht="115.5">
@@ -3843,13 +3855,13 @@
         <v>83</v>
       </c>
       <c r="J272" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K272" s="3" t="s">
         <v>200</v>
       </c>
       <c r="L272" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="273" spans="1:12">
@@ -3857,13 +3869,13 @@
         <v>84</v>
       </c>
       <c r="J273" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K273" t="s">
         <v>201</v>
       </c>
       <c r="L273" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="274" spans="1:12">
@@ -3889,13 +3901,13 @@
         <v>85</v>
       </c>
       <c r="J279" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K279" s="3" t="s">
         <v>204</v>
       </c>
       <c r="L279" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="280" spans="1:12" ht="82.5">
@@ -3903,13 +3915,13 @@
         <v>86</v>
       </c>
       <c r="J280" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K280" s="3" t="s">
         <v>205</v>
       </c>
       <c r="L280" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="281" spans="1:12">
@@ -3917,13 +3929,13 @@
         <v>102</v>
       </c>
       <c r="J281" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K281" t="s">
         <v>206</v>
       </c>
       <c r="L281" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="282" spans="1:12">
@@ -3941,13 +3953,13 @@
         <v>87</v>
       </c>
       <c r="J286" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K286" t="s">
         <v>208</v>
       </c>
       <c r="L286" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="287" spans="1:12" ht="82.5">
@@ -3955,13 +3967,13 @@
         <v>88</v>
       </c>
       <c r="J287" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K287" s="3" t="s">
         <v>209</v>
       </c>
       <c r="L287" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="288" spans="1:12">
@@ -3979,13 +3991,13 @@
         <v>89</v>
       </c>
       <c r="J291" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K291" t="s">
         <v>211</v>
       </c>
       <c r="L291" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="292" spans="1:12" ht="132">
@@ -3993,13 +4005,13 @@
         <v>90</v>
       </c>
       <c r="J292" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="K292" s="3" t="s">
         <v>212</v>
       </c>
       <c r="L292" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="293" spans="1:12">
@@ -4022,13 +4034,13 @@
         <v>91</v>
       </c>
       <c r="J298" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K298" s="3" t="s">
         <v>214</v>
       </c>
       <c r="L298" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="299" spans="1:12" ht="82.5">
@@ -4036,13 +4048,13 @@
         <v>92</v>
       </c>
       <c r="J299" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="K299" s="3" t="s">
         <v>215</v>
       </c>
       <c r="L299" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="300" spans="1:12">
@@ -4076,13 +4088,13 @@
         <v>93</v>
       </c>
       <c r="J305" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K305" s="3" t="s">
         <v>219</v>
       </c>
       <c r="L305" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="306" spans="1:12" ht="165">
@@ -4090,13 +4102,13 @@
         <v>94</v>
       </c>
       <c r="J306" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K306" s="3" t="s">
         <v>220</v>
       </c>
       <c r="L306" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="307" spans="1:12">
@@ -4122,13 +4134,13 @@
         <v>95</v>
       </c>
       <c r="J311" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K311" s="3" t="s">
         <v>223</v>
       </c>
       <c r="L311" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="312" spans="1:12" ht="115.5">
@@ -4136,13 +4148,13 @@
         <v>96</v>
       </c>
       <c r="J312" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K312" s="3" t="s">
         <v>224</v>
       </c>
       <c r="L312" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="313" spans="1:12">
@@ -4165,13 +4177,13 @@
         <v>97</v>
       </c>
       <c r="J317" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K317" s="3" t="s">
         <v>226</v>
       </c>
       <c r="L317" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="319" spans="1:12">
@@ -4189,13 +4201,13 @@
         <v>98</v>
       </c>
       <c r="J323" s="3" t="s">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="K323" s="3" t="s">
         <v>228</v>
       </c>
       <c r="L323" s="3" t="s">
-        <v>347</v>
+        <v>370</v>
       </c>
     </row>
     <row r="324" spans="1:12" ht="148.5">
@@ -4203,13 +4215,13 @@
         <v>99</v>
       </c>
       <c r="J324" s="3" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="K324" s="3" t="s">
         <v>229</v>
       </c>
       <c r="L324" s="3" t="s">
-        <v>348</v>
+        <v>373</v>
       </c>
     </row>
     <row r="325" spans="1:12" ht="82.5">
@@ -4217,13 +4229,13 @@
         <v>100</v>
       </c>
       <c r="J325" s="3" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="K325" s="3" t="s">
         <v>230</v>
       </c>
       <c r="L325" s="3" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
     </row>
     <row r="327" spans="1:12">
@@ -4262,13 +4274,13 @@
         <v>101</v>
       </c>
       <c r="J334" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="K334" s="3" t="s">
         <v>234</v>
       </c>
       <c r="L334" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="335" spans="1:12">
@@ -4294,13 +4306,13 @@
         <v>103</v>
       </c>
       <c r="J341" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="K341" s="4" t="s">
         <v>237</v>
       </c>
       <c r="L341" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="342" spans="1:12" ht="57">
@@ -4308,13 +4320,13 @@
         <v>120</v>
       </c>
       <c r="J342" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="K342" s="4" t="s">
         <v>238</v>
       </c>
       <c r="L342" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="343" spans="1:12">
@@ -4328,13 +4340,13 @@
         <v>121</v>
       </c>
       <c r="J343" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="K343" s="4" t="s">
         <v>240</v>
       </c>
       <c r="L343" s="3" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="344" spans="1:12">
@@ -4348,13 +4360,13 @@
         <v>122</v>
       </c>
       <c r="J344" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="K344" s="4" t="s">
         <v>242</v>
       </c>
       <c r="L344" s="3" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="345" spans="1:12">
@@ -4386,13 +4398,13 @@
         <v>125</v>
       </c>
       <c r="J348" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="K348" s="4" t="s">
         <v>244</v>
       </c>
       <c r="L348" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="349" spans="1:12">
@@ -4420,13 +4432,13 @@
         <v>109</v>
       </c>
       <c r="J350" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="K350" s="4" t="s">
         <v>247</v>
       </c>
       <c r="L350" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="351" spans="1:12" ht="57">
@@ -4437,13 +4449,13 @@
         <v>110</v>
       </c>
       <c r="J351" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="K351" s="4" t="s">
         <v>248</v>
       </c>
       <c r="L351" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="352" spans="1:12">
@@ -4454,13 +4466,13 @@
         <v>104</v>
       </c>
       <c r="J352" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="K352" s="2" t="s">
         <v>249</v>
       </c>
       <c r="L352" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="353" spans="1:12" ht="84">
@@ -4468,13 +4480,13 @@
         <v>105</v>
       </c>
       <c r="J353" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="K353" s="4" t="s">
         <v>250</v>
       </c>
       <c r="L353" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="354" spans="1:12">
@@ -4533,13 +4545,13 @@
         <v>112</v>
       </c>
       <c r="J357" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="K357" s="2" t="s">
         <v>252</v>
       </c>
       <c r="L357" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="358" spans="1:12" ht="18.75">
@@ -4547,13 +4559,13 @@
         <v>113</v>
       </c>
       <c r="J358" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="K358" s="8" t="s">
         <v>253</v>
       </c>
       <c r="L358" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="359" spans="1:12" ht="84">
@@ -4564,13 +4576,13 @@
         <v>114</v>
       </c>
       <c r="J359" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="K359" s="4" t="s">
         <v>254</v>
       </c>
       <c r="L359" s="3" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="360" spans="1:12" ht="124.5">
@@ -4581,13 +4593,13 @@
         <v>115</v>
       </c>
       <c r="J360" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="K360" s="4" t="s">
         <v>255</v>
       </c>
       <c r="L360" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="361" spans="1:12" ht="93.75">
@@ -4595,13 +4607,13 @@
         <v>116</v>
       </c>
       <c r="J361" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="K361" s="9" t="s">
         <v>256</v>
       </c>
       <c r="L361" s="3" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="362" spans="1:12">
@@ -4624,13 +4636,13 @@
         <v>123</v>
       </c>
       <c r="J370" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="K370" t="s">
         <v>257</v>
       </c>
       <c r="L370" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="372" spans="5:12">

</xml_diff>